<commit_message>
Finished hw problems 1-4
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2993A-F70D-6D4C-BBF5-D6F223F8DE52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD851E3-4299-B24C-946F-D380826478A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="4" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="4" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -8496,7 +8496,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>CIZV-3821-0002</v>
+        <v>QVFO-8467-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8506,11 +8506,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39011</v>
+        <v>38803</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>51183</v>
+        <v>44201</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10210,7 +10210,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>RUWD-8305-0002</v>
+        <v>TLNT-5384-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10220,11 +10220,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>38140</v>
+        <v>37221</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>33692</v>
+        <v>42169</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -13284,7 +13284,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D6" sqref="D6:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13336,9 +13336,9 @@
       <c r="C6" s="6">
         <v>131.07</v>
       </c>
-      <c r="D6" s="8" t="e">
-        <f>HLOOKUP(B6,$H$7:$I$9,MATCH(B6,H7:H9))</f>
-        <v>#N/A</v>
+      <c r="D6" s="8" t="str">
+        <f>INDEX($I$7:$I$9, MATCH(B6, $H$7:$H$9,0))</f>
+        <v>OUTDOOR-1570</v>
       </c>
       <c r="H6" s="36" t="s">
         <v>531</v>
@@ -13358,7 +13358,10 @@
       <c r="C7" s="6">
         <v>159.47999999999999</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8" t="str">
+        <f t="shared" ref="D7:D24" si="0">INDEX($I$7:$I$9, MATCH(B7, $H$7:$H$9,0))</f>
+        <v>OUTDOOR-1570</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>532</v>
       </c>
@@ -13376,7 +13379,10 @@
       <c r="C8" s="6">
         <v>84.98</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>534</v>
       </c>
@@ -13394,7 +13400,10 @@
       <c r="C9" s="6">
         <v>85.33</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>530</v>
       </c>
@@ -13412,7 +13421,10 @@
       <c r="C10" s="6">
         <v>109.55</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -13424,7 +13436,10 @@
       <c r="C11" s="6">
         <v>151.96</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -13436,7 +13451,10 @@
       <c r="C12" s="6">
         <v>87.65</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -13448,7 +13466,10 @@
       <c r="C13" s="6">
         <v>135.76</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -13460,10 +13481,9 @@
       <c r="C14" s="6">
         <v>153.51</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="H14" t="e">
-        <f>INDEX($B$4:$H$4,MATCH(I5,B5:H5,0))</f>
-        <v>#N/A</v>
+      <c r="D14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAD-1084</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -13476,7 +13496,10 @@
       <c r="C15" s="6">
         <v>113.04</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -13488,7 +13511,10 @@
       <c r="C16" s="6">
         <v>138.41999999999999</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
@@ -13500,7 +13526,10 @@
       <c r="C17" s="6">
         <v>154.69</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
@@ -13512,7 +13541,10 @@
       <c r="C18" s="6">
         <v>145.99</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
@@ -13524,7 +13556,10 @@
       <c r="C19" s="6">
         <v>97.45</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
@@ -13536,7 +13571,10 @@
       <c r="C20" s="6">
         <v>130.43</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
@@ -13548,7 +13586,10 @@
       <c r="C21" s="6">
         <v>118.56</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
@@ -13560,7 +13601,10 @@
       <c r="C22" s="6">
         <v>127.48</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
@@ -13572,7 +13616,10 @@
       <c r="C23" s="6">
         <v>95.27</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="8" t="str">
+        <f>INDEX($I$7:$I$9, MATCH(B23, $H$7:$H$9,0))</f>
+        <v>OUTDOOR-1570</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
@@ -13584,7 +13631,10 @@
       <c r="C24" s="6">
         <v>146.35</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished hw problem 5
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD851E3-4299-B24C-946F-D380826478A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D292E1E-1B6A-EC47-B8AD-CD960098C2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="4" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="848">
   <si>
     <t>Boomerang</t>
   </si>
@@ -3771,6 +3771,9 @@
   </si>
   <si>
     <t>How to use VLOOKUP, LEFT and SEARCH to do a "Partial Text Lookup. Goal: Lookup Product Price. Also: Look at Data Mismatch in lookup formulas.</t>
+  </si>
+  <si>
+    <t>w/Vlookup</t>
   </si>
 </sst>
 </file>
@@ -4177,7 +4180,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4358,6 +4361,12 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -8496,7 +8505,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>QVFO-8467-0002</v>
+        <v>WUJR-4958-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8506,11 +8515,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>38803</v>
+        <v>39984</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>44201</v>
+        <v>58468</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10210,7 +10219,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>TLNT-5384-0002</v>
+        <v>MHXT-8124-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10220,11 +10229,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37221</v>
+        <v>39849</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>42169</v>
+        <v>34600</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -13283,8 +13292,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D24"/>
+    <sheetView topLeftCell="A3" zoomScale="161" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13292,6 +13301,7 @@
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -13323,6 +13333,9 @@
       <c r="D5" s="4" t="s">
         <v>529</v>
       </c>
+      <c r="E5" s="123" t="s">
+        <v>847</v>
+      </c>
       <c r="H5" s="36"/>
       <c r="I5" s="36"/>
     </row>
@@ -13340,6 +13353,10 @@
         <f>INDEX($I$7:$I$9, MATCH(B6, $H$7:$H$9,0))</f>
         <v>OUTDOOR-1570</v>
       </c>
+      <c r="E6" t="str">
+        <f>VLOOKUP(B6, $H$7:$I$9, 2, 0)</f>
+        <v>OUTDOOR-1570</v>
+      </c>
       <c r="H6" s="36" t="s">
         <v>531</v>
       </c>
@@ -13362,6 +13379,10 @@
         <f t="shared" ref="D7:D24" si="0">INDEX($I$7:$I$9, MATCH(B7, $H$7:$H$9,0))</f>
         <v>OUTDOOR-1570</v>
       </c>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:E24" si="1">VLOOKUP(B7, $H$7:$I$9, 2, 0)</f>
+        <v>OUTDOOR-1570</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>532</v>
       </c>
@@ -13383,6 +13404,10 @@
         <f t="shared" si="0"/>
         <v>SPORT-1876</v>
       </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>SPORT-1876</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>534</v>
       </c>
@@ -13404,6 +13429,10 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>530</v>
       </c>
@@ -13425,6 +13454,10 @@
         <f t="shared" si="0"/>
         <v>SPORT-1876</v>
       </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -13440,6 +13473,10 @@
         <f t="shared" si="0"/>
         <v>RAD-1084</v>
       </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -13455,6 +13492,10 @@
         <f t="shared" si="0"/>
         <v>RAD-1084</v>
       </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -13470,6 +13511,10 @@
         <f t="shared" si="0"/>
         <v>SPORT-1876</v>
       </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>SPORT-1876</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -13485,6 +13530,10 @@
         <f t="shared" si="0"/>
         <v>RAD-1084</v>
       </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -13500,6 +13549,10 @@
         <f t="shared" si="0"/>
         <v>RAD-1084</v>
       </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>RAD-1084</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -13515,8 +13568,12 @@
         <f t="shared" si="0"/>
         <v>SPORT-1876</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>SPORT-1876</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>40325</v>
       </c>
@@ -13530,8 +13587,12 @@
         <f t="shared" si="0"/>
         <v>RAD-1084</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="str">
+        <f>VLOOKUP(B17, $H$7:$I$9, 2, 0)</f>
+        <v>RAD-1084</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>40326</v>
       </c>
@@ -13545,8 +13606,12 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>40327</v>
       </c>
@@ -13560,8 +13625,12 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>40328</v>
       </c>
@@ -13575,8 +13644,12 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>40329</v>
       </c>
@@ -13590,8 +13663,12 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>40330</v>
       </c>
@@ -13605,8 +13682,12 @@
         <f t="shared" si="0"/>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>40331</v>
       </c>
@@ -13620,8 +13701,12 @@
         <f>INDEX($I$7:$I$9, MATCH(B23, $H$7:$H$9,0))</f>
         <v>OUTDOOR-1570</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>OUTDOOR-1570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>40332</v>
       </c>
@@ -13633,6 +13718,10 @@
       </c>
       <c r="D24" s="8" t="str">
         <f t="shared" si="0"/>
+        <v>SPORT-1876</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
         <v>SPORT-1876</v>
       </c>
     </row>
@@ -16631,8 +16720,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16996,8 +17085,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17058,8 +17147,14 @@
         <v>539</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="16"/>
+      <c r="G3" s="132" t="str">
+        <f>INDEX(A3:A8, MATCH($E$3,$C$3:$C$8,0))</f>
+        <v>Quad</v>
+      </c>
+      <c r="H3" s="133">
+        <f>INDEX(B3:B8, MATCH($E$3,$C$3:$C$8,0))</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">

</xml_diff>

<commit_message>
Finished hw problem 6
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D292E1E-1B6A-EC47-B8AD-CD960098C2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD57B33-A557-4140-BAAE-41AB0EA8F694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>WUJR-4958-0002</v>
+        <v>YVUF-2748-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8515,11 +8515,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39984</v>
+        <v>39868</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>58468</v>
+        <v>45088</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10219,7 +10219,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>MHXT-8124-0002</v>
+        <v>YJGC-9193-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10229,11 +10229,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39849</v>
+        <v>37456</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>34600</v>
+        <v>38613</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -17085,7 +17085,7 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -17229,7 +17229,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17371,8 +17371,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17447,7 +17447,10 @@
       <c r="E4" s="90" t="s">
         <v>551</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8">
+        <f>IF(D4="ProductLine1",INDEX($I$4:$I$7,MATCH(C4,$H$4:$H$7,0)),INDEX($L$4:$L$7,MATCH(C4,$K$4:$K$7,0)))</f>
+        <v>125</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>552</v>
       </c>
@@ -17477,7 +17480,10 @@
       <c r="E5" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8">
+        <f t="shared" ref="F5:F24" si="0">IF(D5="ProductLine1",INDEX($I$4:$I$7,MATCH(C5,$H$4:$H$7,0)),INDEX($L$4:$L$7,MATCH(C5,$K$4:$K$7,0)))</f>
+        <v>125</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>555</v>
       </c>
@@ -17507,7 +17513,10 @@
       <c r="E6" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>549</v>
       </c>
@@ -17537,7 +17546,10 @@
       <c r="E7" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>557</v>
       </c>
@@ -17567,7 +17579,10 @@
       <c r="E8" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.75E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
@@ -17585,7 +17600,10 @@
       <c r="E9" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
@@ -17603,7 +17621,10 @@
       <c r="E10" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -17621,7 +17642,10 @@
       <c r="E11" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -17639,7 +17663,10 @@
       <c r="E12" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -17657,7 +17684,10 @@
       <c r="E13" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -17675,7 +17705,10 @@
       <c r="E14" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -17693,7 +17726,10 @@
       <c r="E15" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -17711,7 +17747,10 @@
       <c r="E16" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
@@ -17729,7 +17768,10 @@
       <c r="E17" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
@@ -17747,7 +17789,10 @@
       <c r="E18" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
@@ -17765,7 +17810,10 @@
       <c r="E19" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
@@ -17783,7 +17831,10 @@
       <c r="E20" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
@@ -17801,7 +17852,10 @@
       <c r="E21" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
@@ -17819,7 +17873,10 @@
       <c r="E22" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
@@ -17837,7 +17894,10 @@
       <c r="E23" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
@@ -17855,7 +17915,10 @@
       <c r="E24" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E25" s="91"/>
@@ -17873,7 +17936,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed hw problem 6
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD57B33-A557-4140-BAAE-41AB0EA8F694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8815C9-5DF3-FA47-BF0B-BA42C45C601F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="849">
   <si>
     <t>Boomerang</t>
   </si>
@@ -3774,6 +3774,9 @@
   </si>
   <si>
     <t>w/Vlookup</t>
+  </si>
+  <si>
+    <t>w/ Vlookup</t>
   </si>
 </sst>
 </file>
@@ -4180,7 +4183,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4369,6 +4372,7 @@
     <xf numFmtId="167" fontId="0" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -8505,7 +8509,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>YVUF-2748-0002</v>
+        <v>URXP-4907-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8515,11 +8519,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39868</v>
+        <v>37938</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>45088</v>
+        <v>56099</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10219,7 +10223,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>YJGC-9193-0002</v>
+        <v>NBCR-6970-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10229,11 +10233,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37456</v>
+        <v>39580</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>38613</v>
+        <v>57516</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -17372,7 +17376,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F24"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17383,6 +17387,7 @@
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
@@ -17422,6 +17427,9 @@
       <c r="F3" s="28" t="s">
         <v>216</v>
       </c>
+      <c r="G3" s="134" t="s">
+        <v>848</v>
+      </c>
       <c r="H3" s="88" t="s">
         <v>547</v>
       </c>
@@ -17448,7 +17456,7 @@
         <v>551</v>
       </c>
       <c r="F4" s="8">
-        <f>IF(D4="ProductLine1",INDEX($I$4:$I$7,MATCH(C4,$H$4:$H$7,0)),INDEX($L$4:$L$7,MATCH(C4,$K$4:$K$7,0)))</f>
+        <f>IF(D4="ProductLine1",INDEX($I$4:$I$7,MATCH(C4,$H$4:$H$7,0)),(B4*INDEX($L$4:$L$7,MATCH(C4,$K$4:$K$7,0))))</f>
         <v>125</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -17481,7 +17489,7 @@
         <v>554</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" ref="F5:F24" si="0">IF(D5="ProductLine1",INDEX($I$4:$I$7,MATCH(C5,$H$4:$H$7,0)),INDEX($L$4:$L$7,MATCH(C5,$K$4:$K$7,0)))</f>
+        <f t="shared" ref="F5:F24" si="0">IF(D5="ProductLine1",INDEX($I$4:$I$7,MATCH(C5,$H$4:$H$7,0)),(B5*INDEX($L$4:$L$7,MATCH(C5,$K$4:$K$7,0))))</f>
         <v>125</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -17548,7 +17556,7 @@
       </c>
       <c r="F7" s="8">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>87.873400000000004</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>557</v>
@@ -17581,7 +17589,7 @@
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
-        <v>2.75E-2</v>
+        <v>123.18900000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -17602,7 +17610,7 @@
       </c>
       <c r="F9" s="8">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>53.099600000000002</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -17623,7 +17631,7 @@
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>99.855500000000006</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -17665,7 +17673,7 @@
       </c>
       <c r="F12" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>142.03020000000001</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -17728,7 +17736,7 @@
       </c>
       <c r="F15" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>142.99199999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -17770,7 +17778,7 @@
       </c>
       <c r="F17" s="8">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>106.81700000000001</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -17812,7 +17820,7 @@
       </c>
       <c r="F19" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>131.6799</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -17896,7 +17904,7 @@
       </c>
       <c r="F23" s="8">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>55.460600000000007</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -17917,7 +17925,7 @@
       </c>
       <c r="F24" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>64.365300000000005</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed hw problem 7
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8815C9-5DF3-FA47-BF0B-BA42C45C601F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DCCB6D-30D2-5440-A2C1-226D50F33831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="11" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="849">
   <si>
     <t>Boomerang</t>
   </si>
@@ -4183,7 +4183,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4373,6 +4373,7 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -8509,7 +8510,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>URXP-4907-0002</v>
+        <v>QZEP-3220-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8519,11 +8520,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37938</v>
+        <v>40266</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>56099</v>
+        <v>56105</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10223,7 +10224,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>NBCR-6970-0002</v>
+        <v>FDRN-5401-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10233,11 +10234,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39580</v>
+        <v>37462</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>57516</v>
+        <v>45961</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -17375,8 +17376,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17459,6 +17460,10 @@
         <f>IF(D4="ProductLine1",INDEX($I$4:$I$7,MATCH(C4,$H$4:$H$7,0)),(B4*INDEX($L$4:$L$7,MATCH(C4,$K$4:$K$7,0))))</f>
         <v>125</v>
       </c>
+      <c r="G4">
+        <f>IF(D4="ProductLine1",VLOOKUP(C4,$H$4:$I$7,2,TRUE),B4*VLOOKUP(C4,$K$4:$L$7,2,0))</f>
+        <v>125</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>552</v>
       </c>
@@ -17492,6 +17497,10 @@
         <f t="shared" ref="F5:F24" si="0">IF(D5="ProductLine1",INDEX($I$4:$I$7,MATCH(C5,$H$4:$H$7,0)),(B5*INDEX($L$4:$L$7,MATCH(C5,$K$4:$K$7,0))))</f>
         <v>125</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G24" si="1">IF(D5="ProductLine1",VLOOKUP(C5,$H$4:$I$7,2,TRUE),B5*VLOOKUP(C5,$K$4:$L$7,2,0))</f>
+        <v>125</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>555</v>
       </c>
@@ -17525,6 +17534,10 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>549</v>
       </c>
@@ -17558,6 +17571,10 @@
         <f t="shared" si="0"/>
         <v>87.873400000000004</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>87.873400000000004</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>557</v>
       </c>
@@ -17591,6 +17608,10 @@
         <f t="shared" si="0"/>
         <v>123.18900000000001</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>123.18900000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
@@ -17612,6 +17633,10 @@
         <f t="shared" si="0"/>
         <v>53.099600000000002</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>53.099600000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
@@ -17633,6 +17658,10 @@
         <f t="shared" si="0"/>
         <v>99.855500000000006</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>99.855500000000006</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -17654,6 +17683,10 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -17675,6 +17708,10 @@
         <f t="shared" si="0"/>
         <v>142.03020000000001</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>142.03020000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -17696,6 +17733,10 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -17717,6 +17758,10 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -17738,6 +17783,10 @@
         <f t="shared" si="0"/>
         <v>142.99199999999999</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>142.99199999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -17759,8 +17808,12 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>40328</v>
       </c>
@@ -17780,8 +17833,12 @@
         <f t="shared" si="0"/>
         <v>106.81700000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>106.81700000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>40329</v>
       </c>
@@ -17801,8 +17858,12 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>40330</v>
       </c>
@@ -17822,8 +17883,12 @@
         <f t="shared" si="0"/>
         <v>131.6799</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>131.6799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>40331</v>
       </c>
@@ -17843,8 +17908,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>40332</v>
       </c>
@@ -17864,8 +17933,12 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>40333</v>
       </c>
@@ -17885,8 +17958,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>40334</v>
       </c>
@@ -17906,8 +17983,12 @@
         <f t="shared" si="0"/>
         <v>55.460600000000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>55.460600000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>40335</v>
       </c>
@@ -17927,8 +18008,12 @@
         <f t="shared" si="0"/>
         <v>64.365300000000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>64.365300000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E25" s="91"/>
     </row>
   </sheetData>
@@ -17943,7 +18028,7 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -18507,8 +18592,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18554,6 +18639,9 @@
       <c r="F3" s="28" t="s">
         <v>216</v>
       </c>
+      <c r="G3" s="134" t="s">
+        <v>847</v>
+      </c>
       <c r="I3" s="88" t="s">
         <v>581</v>
       </c>
@@ -18579,7 +18667,14 @@
       <c r="E4" s="90" t="s">
         <v>551</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="135">
+        <f>IF(D4="ProductLine1", B4* INDEX($J$4:$J$7, MATCH(C4,$I$4:$I$7,0)), B4*INDEX($M$4:$M$7, MATCH(C4,$L$4:$L$7,0)))</f>
+        <v>128.5684</v>
+      </c>
+      <c r="G4">
+        <f>IF(D4="ProductLine1",B4*VLOOKUP(C4,$I$4:$J$7,2,FALSE),B4*VLOOKUP(C4,$L$4:$M$7,2,FALSE))</f>
+        <v>128.5684</v>
+      </c>
       <c r="I4" s="5" t="s">
         <v>552</v>
       </c>
@@ -18609,7 +18704,14 @@
       <c r="E5" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="135">
+        <f t="shared" ref="F5:F24" si="0">IF(D5="ProductLine1", B5* INDEX($J$4:$J$7, MATCH(C5,$I$4:$I$7,0)), B5*INDEX($M$4:$M$7, MATCH(C5,$L$4:$L$7,0)))</f>
+        <v>113.58320000000001</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G24" si="1">IF(D5="ProductLine1",B5*VLOOKUP(C5,$I$4:$J$7,2,FALSE),B5*VLOOKUP(C5,$L$4:$M$7,2,FALSE))</f>
+        <v>113.58320000000001</v>
+      </c>
       <c r="I5" s="5" t="s">
         <v>555</v>
       </c>
@@ -18639,7 +18741,14 @@
       <c r="E6" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="135">
+        <f t="shared" si="0"/>
+        <v>204.02350000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>204.02350000000001</v>
+      </c>
       <c r="I6" s="5" t="s">
         <v>549</v>
       </c>
@@ -18669,7 +18778,14 @@
       <c r="E7" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="135">
+        <f t="shared" si="0"/>
+        <v>87.873400000000004</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>87.873400000000004</v>
+      </c>
       <c r="I7" s="5" t="s">
         <v>557</v>
       </c>
@@ -18699,7 +18815,14 @@
       <c r="E8" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="135">
+        <f t="shared" si="0"/>
+        <v>123.18900000000001</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>123.18900000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
@@ -18717,7 +18840,14 @@
       <c r="E9" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="135">
+        <f t="shared" si="0"/>
+        <v>53.099600000000002</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>53.099600000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
@@ -18735,7 +18865,14 @@
       <c r="E10" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="135">
+        <f t="shared" si="0"/>
+        <v>99.855500000000006</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>99.855500000000006</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -18753,7 +18890,14 @@
       <c r="E11" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="135">
+        <f t="shared" si="0"/>
+        <v>143.45800000000003</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>143.45800000000003</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -18771,7 +18915,14 @@
       <c r="E12" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="135">
+        <f t="shared" si="0"/>
+        <v>142.03020000000001</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>142.03020000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -18789,7 +18940,14 @@
       <c r="E13" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="135">
+        <f t="shared" si="0"/>
+        <v>104.79299999999999</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>104.79299999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -18807,7 +18965,14 @@
       <c r="E14" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="135">
+        <f t="shared" si="0"/>
+        <v>114.95085</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>114.95085</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -18825,7 +18990,14 @@
       <c r="E15" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="135">
+        <f t="shared" si="0"/>
+        <v>142.99199999999999</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>142.99199999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -18843,9 +19015,16 @@
       <c r="E16" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="135">
+        <f t="shared" si="0"/>
+        <v>144.06440000000001</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>144.06440000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>40328</v>
       </c>
@@ -18861,9 +19040,16 @@
       <c r="E17" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="135">
+        <f t="shared" si="0"/>
+        <v>106.81700000000001</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>106.81700000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>40329</v>
       </c>
@@ -18879,9 +19065,16 @@
       <c r="E18" s="5" t="s">
         <v>573</v>
       </c>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="135">
+        <f t="shared" si="0"/>
+        <v>85.707599999999999</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>85.707599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>40330</v>
       </c>
@@ -18897,9 +19090,16 @@
       <c r="E19" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="135">
+        <f t="shared" si="0"/>
+        <v>131.6799</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>131.6799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>40331</v>
       </c>
@@ -18915,9 +19115,16 @@
       <c r="E20" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="135">
+        <f t="shared" si="0"/>
+        <v>193.809</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>193.809</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>40332</v>
       </c>
@@ -18933,9 +19140,16 @@
       <c r="E21" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="135">
+        <f t="shared" si="0"/>
+        <v>136.76985000000002</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>136.76985000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>40333</v>
       </c>
@@ -18951,9 +19165,16 @@
       <c r="E22" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="135">
+        <f t="shared" si="0"/>
+        <v>207.535</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>207.535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>40334</v>
       </c>
@@ -18969,9 +19190,16 @@
       <c r="E23" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="135">
+        <f t="shared" si="0"/>
+        <v>55.460600000000007</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>55.460600000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>40335</v>
       </c>
@@ -18987,9 +19215,16 @@
       <c r="E24" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="135">
+        <f t="shared" si="0"/>
+        <v>64.365300000000005</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>64.365300000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E25" s="91"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed hw problem 8
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DCCB6D-30D2-5440-A2C1-226D50F33831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1258FFDA-61C5-1E42-AC5F-77497632A401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="11" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="12" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -8510,7 +8510,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>QZEP-3220-0002</v>
+        <v>BYXT-4771-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8520,11 +8520,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>40266</v>
+        <v>37752</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>56105</v>
+        <v>29014</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10224,7 +10224,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>FDRN-5401-0002</v>
+        <v>DIUJ-6543-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10234,11 +10234,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37462</v>
+        <v>37646</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>45961</v>
+        <v>36720</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -18592,7 +18592,7 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G24"/>
     </sheetView>
   </sheetViews>
@@ -19886,8 +19886,8 @@
   </sheetPr>
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19923,7 +19923,10 @@
       <c r="A4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="16">
+        <f>SUM(INDEX($A$6:$L$93,,MATCH($B$3, $A$6:$L$6, 0)))</f>
+        <v>702351</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -23288,7 +23291,7 @@
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26674,7 +26677,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1B00-000000000000}">
       <formula1>$A$6:$L$6</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Finished hw problem 9
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1258FFDA-61C5-1E42-AC5F-77497632A401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36455095-D8F5-F446-9A59-BDD6D3D7976F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="12" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="15" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="850">
   <si>
     <t>Boomerang</t>
   </si>
@@ -3777,6 +3777,9 @@
   </si>
   <si>
     <t>w/ Vlookup</t>
+  </si>
+  <si>
+    <t>Cost of each product sold</t>
   </si>
 </sst>
 </file>
@@ -8510,7 +8513,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>BYXT-4771-0002</v>
+        <v>UNUC-4446-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8520,11 +8523,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37752</v>
+        <v>39961</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>29014</v>
+        <v>31244</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10224,7 +10227,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>DIUJ-6543-0002</v>
+        <v>LYXX-7932-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10234,11 +10237,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37646</v>
+        <v>37587</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>36720</v>
+        <v>54052</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -19886,7 +19889,7 @@
   </sheetPr>
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="118" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -26692,16 +26695,17 @@
   <sheetPr>
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26727,6 +26731,9 @@
       <c r="B4" s="4" t="s">
         <v>608</v>
       </c>
+      <c r="C4" t="s">
+        <v>849</v>
+      </c>
       <c r="H4" s="116" t="s">
         <v>610</v>
       </c>
@@ -26739,6 +26746,10 @@
       <c r="B5" s="5" t="s">
         <v>510</v>
       </c>
+      <c r="C5">
+        <f>VLOOKUP(B5,$H$6:$I$8,2)</f>
+        <v>12.5</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
@@ -26753,6 +26764,10 @@
       <c r="B6" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C26" si="0">VLOOKUP(B6,$H$6:$I$8,2)</f>
+        <v>5.75</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>510</v>
       </c>
@@ -26767,6 +26782,10 @@
       <c r="B7" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>511</v>
       </c>
@@ -26781,6 +26800,10 @@
       <c r="B8" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>512</v>
       </c>
@@ -26795,6 +26818,10 @@
       <c r="B9" s="5" t="s">
         <v>511</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
@@ -26803,6 +26830,10 @@
       <c r="B10" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
@@ -26811,6 +26842,10 @@
       <c r="B11" s="5" t="s">
         <v>510</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
@@ -26819,6 +26854,10 @@
       <c r="B12" s="5" t="s">
         <v>511</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
@@ -26827,6 +26866,10 @@
       <c r="B13" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
@@ -26835,6 +26878,10 @@
       <c r="B14" s="5" t="s">
         <v>511</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
@@ -26843,6 +26890,10 @@
       <c r="B15" s="5" t="s">
         <v>512</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
@@ -26851,85 +26902,135 @@
       <c r="B16" s="5" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>42491</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>42491</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>42497</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>42495</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>42499</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>42499</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>42494</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>42498</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>42502</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>42498</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>512</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f>SUM(C5:C26)</f>
+        <v>239.75</v>
       </c>
     </row>
   </sheetData>
@@ -30133,7 +30234,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30501,7 +30602,7 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished all HW problems
</commit_message>
<xml_diff>
--- a/Busn218-Video11_edit.xlsx
+++ b/Busn218-Video11_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/vlookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36455095-D8F5-F446-9A59-BDD6D3D7976F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544EA5E8-8FBB-6142-8D01-9B213CC7471A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="15" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="16" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="25" r:id="rId1"/>
@@ -8513,7 +8513,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>UNUC-4446-0002</v>
+        <v>TKWQ-4769-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -8523,11 +8523,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>39961</v>
+        <v>37498</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>31244</v>
+        <v>42889</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -10227,7 +10227,7 @@
       </c>
       <c r="AA3" t="str">
         <f ca="1">CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;CHAR(65+INT(RAND()*25+1))&amp;"-"&amp;RANDBETWEEN(1000,9999)&amp;"-"&amp;TEXT(ROWS(AA$2:AA3),"0000")</f>
-        <v>LYXX-7932-0002</v>
+        <v>HDYF-5942-0002</v>
       </c>
       <c r="AB3" t="s">
         <v>247</v>
@@ -10237,11 +10237,11 @@
       </c>
       <c r="AD3" s="74">
         <f t="shared" ref="AD3" ca="1" si="0">RANDBETWEEN(37000,40300)</f>
-        <v>37587</v>
+        <v>38694</v>
       </c>
       <c r="AE3" s="69">
         <f ca="1">RANDBETWEEN(29000,59000)</f>
-        <v>54052</v>
+        <v>48293</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -30602,8 +30602,8 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30656,8 +30656,14 @@
       <c r="C6" s="5" t="s">
         <v>783</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="D6" s="8" t="b">
+        <f>ISNUMBER(MATCH(C6, $A$6:$A$15, 0))</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <f>ISNA(MATCH(C6,$A$6:$A$15,0))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -30666,8 +30672,14 @@
       <c r="C7" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="D7" s="8" t="b">
+        <f t="shared" ref="D7:D13" si="0">ISNUMBER(MATCH(C7, $A$6:$A$15, 0))</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="b">
+        <f t="shared" ref="G7:G13" si="1">ISNA(MATCH(C7,$A$6:$A$15,0))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -30676,8 +30688,14 @@
       <c r="C8" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="D8" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -30686,8 +30704,14 @@
       <c r="C9" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -30696,8 +30720,14 @@
       <c r="C10" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -30706,8 +30736,14 @@
       <c r="C11" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="D11" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -30716,8 +30752,14 @@
       <c r="C12" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -30726,8 +30768,14 @@
       <c r="C13" s="5" t="s">
         <v>793</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="D13" s="8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">

</xml_diff>